<commit_message>
Fixed formatting on community evals
</commit_message>
<xml_diff>
--- a/eld_cube_prospective/ELD_Testing_Cube_Community.xlsx
+++ b/eld_cube_prospective/ELD_Testing_Cube_Community.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jettcrowdis/Documents/github/tireless-tracker/eld_cube_prospective/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060EA313-A90F-F747-B075-4A93AF04756C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7279EA8E-A66D-AE4D-AD6B-D5F3539B3FEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="460" windowWidth="28020" windowHeight="16600" xr2:uid="{898F8FB1-E390-734B-9F3C-7B39216D8A09}"/>
   </bookViews>
@@ -687,11 +687,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1009,250 +1012,313 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4603A77-796F-644F-9445-05A47A87EC71}">
   <dimension ref="A1:BH44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BG2" sqref="BG2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AQ14" sqref="AQ14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="33" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="54" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="53.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="2.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="4"/>
+      <c r="M1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="4"/>
+      <c r="O1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1" t="s">
+      <c r="R1" s="4"/>
+      <c r="S1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1" t="s">
+      <c r="T1" s="4"/>
+      <c r="U1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="V1" s="4"/>
+      <c r="W1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1" t="s">
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1" t="s">
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1" t="s">
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1" t="s">
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1" t="s">
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1" t="s">
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1" t="s">
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1" t="s">
+      <c r="AL1" s="4"/>
+      <c r="AM1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1" t="s">
+      <c r="AN1" s="4"/>
+      <c r="AO1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1" t="s">
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1" t="s">
+      <c r="AR1" s="4"/>
+      <c r="AS1" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1" t="s">
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1" t="s">
+      <c r="AV1" s="4"/>
+      <c r="AW1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="AX1" s="1"/>
-      <c r="AY1" s="1" t="s">
+      <c r="AX1" s="4"/>
+      <c r="AY1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AZ1" s="1"/>
-      <c r="BA1" s="1" t="s">
+      <c r="AZ1" s="4"/>
+      <c r="BA1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="BB1" s="1"/>
-      <c r="BC1" t="s">
+      <c r="BB1" s="4"/>
+      <c r="BC1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BD1" s="4"/>
+      <c r="BE1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BF1" s="4"/>
+      <c r="BG1" s="4" t="s">
         <v>201</v>
       </c>
+      <c r="BH1" s="4"/>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1" t="s">
+      <c r="R2" s="4"/>
+      <c r="S2" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1" t="s">
+      <c r="V2" s="4"/>
+      <c r="W2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1" t="s">
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1" t="s">
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1" t="s">
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1" t="s">
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1" t="s">
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1" t="s">
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1" t="s">
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+      <c r="AP2" s="4"/>
+      <c r="AQ2" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1" t="s">
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1" t="s">
+      <c r="AT2" s="4"/>
+      <c r="AU2" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AV2" s="1"/>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1" t="s">
+      <c r="AV2" s="4"/>
+      <c r="AW2" s="4"/>
+      <c r="AX2" s="4"/>
+      <c r="AY2" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="AZ2" s="1"/>
-      <c r="BA2" s="1" t="s">
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="BB2" s="1"/>
-      <c r="BC2" t="s">
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BF2" s="4"/>
+      <c r="BG2" s="4" t="s">
         <v>188</v>
       </c>
+      <c r="BH2" s="4"/>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -4809,6 +4875,68 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="60">
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AY2:AZ2"/>
+    <mergeCell ref="BA2:BB2"/>
+    <mergeCell ref="BC2:BD2"/>
+    <mergeCell ref="BE2:BF2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="AY1:AZ1"/>
+    <mergeCell ref="BA1:BB1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="BE1:BF1"/>
+    <mergeCell ref="BG1:BH1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AS1:AT1"/>
+    <mergeCell ref="AU1:AV1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{B0E63802-1177-754E-B8B6-6E6AAF2746E1}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{7307C520-C371-764D-9698-46005E871CEE}"/>

</xml_diff>